<commit_message>
actulizacion historia de usuario
</commit_message>
<xml_diff>
--- a/Desarrollo/Carta Digital/1. REQUERIMIENTOS SCRUM/CD-CP.xlsx
+++ b/Desarrollo/Carta Digital/1. REQUERIMIENTOS SCRUM/CD-CP.xlsx
@@ -332,7 +332,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -381,7 +381,6 @@
     </font>
     <font>
       <sz val="12.0"/>
-      <color theme="1"/>
       <name val="Century Gothic"/>
     </font>
     <font>
@@ -393,6 +392,11 @@
       <sz val="12.0"/>
       <color theme="1"/>
       <name val="&quot;Century Gothic&quot;"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -480,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -555,10 +559,13 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1122,7 +1129,7 @@
         <v>44361.0</v>
       </c>
       <c r="G19" s="19">
-        <v>44379.0</v>
+        <v>44387.0</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -1291,14 +1298,14 @@
       <c r="F28" s="28">
         <v>44375.0</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="29">
         <v>44376.0</v>
       </c>
       <c r="H28" s="18"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="15"/>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="30" t="s">
         <v>72</v>
       </c>
       <c r="C29" s="18"/>
@@ -1343,7 +1350,7 @@
       <c r="H31" s="18"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="31" t="s">
         <v>78</v>
       </c>
       <c r="C32" s="18"/>
@@ -1358,7 +1365,7 @@
         <v>79</v>
       </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="32" t="s">
         <v>80</v>
       </c>
       <c r="E33" s="14" t="s">
@@ -1415,7 +1422,7 @@
         <v>86</v>
       </c>
       <c r="C36" s="18"/>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="32" t="s">
         <v>87</v>
       </c>
       <c r="E36" s="14" t="s">
@@ -1430,7 +1437,7 @@
       <c r="H36" s="18"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="33" t="s">
         <v>88</v>
       </c>
       <c r="C37" s="18"/>
@@ -1457,7 +1464,7 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="15"/>
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="34" t="s">
         <v>90</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -1479,7 +1486,7 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="15"/>
-      <c r="B40" s="34" t="s">
+      <c r="B40" s="35" t="s">
         <v>92</v>
       </c>
       <c r="C40" s="9"/>
@@ -1491,7 +1498,7 @@
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="15"/>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="36" t="s">
         <v>93</v>
       </c>
       <c r="C41" s="9"/>
@@ -1503,7 +1510,7 @@
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="15"/>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="37" t="s">
         <v>94</v>
       </c>
       <c r="C42" s="9"/>
@@ -1515,7 +1522,7 @@
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="15"/>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="36" t="s">
         <v>95</v>
       </c>
       <c r="C43" s="9"/>
@@ -1571,7 +1578,7 @@
       <c r="H46" s="18"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="B47" s="37" t="s">
+      <c r="B47" s="38" t="s">
         <v>100</v>
       </c>
       <c r="C47" s="18"/>

</xml_diff>